<commit_message>
Small changes for consitency and format
</commit_message>
<xml_diff>
--- a/src/files/ERP.xlsx
+++ b/src/files/ERP.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rb.win.frb.org\B1\Accounts\RE\D-F\B1FXD02\Redirected\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcefxd02\Dropbox\fernandoduarte.github.io\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5220400-3A0D-4704-B164-31274F388ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028D261E-DDE8-4BC1-A776-DFB059409D4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ERP_vintages" sheetId="1" r:id="rId1"/>
+    <sheet name="ERP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>